<commit_message>
New Mexico Aggregate data update.
New Mexico Aggregate data update.  Standardized code, water source type date.
</commit_message>
<xml_diff>
--- a/NewMexico/AggregatedAmounts/NM_Aggregated Schema Mapping to WaDE_QA.xlsx
+++ b/NewMexico/AggregatedAmounts/NM_Aggregated Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\NewMexico\AggregatedAmounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC3B97D-F15B-42E7-884B-F775EFABFDD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8093F337-DCAB-42BD-9722-8186BA80A011}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="645" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="645" activeTab="4" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="257">
   <si>
     <t>Name</t>
   </si>
@@ -728,13 +728,7 @@
     <t>NMOSE_Water Uses</t>
   </si>
   <si>
-    <t>NMOSE_Consumptive Use</t>
-  </si>
-  <si>
     <t>AF</t>
-  </si>
-  <si>
-    <t>Rebecca Mitchell</t>
   </si>
   <si>
     <t>https://github.com/WSWCWaterDataExchange/MappingStatesDataToWaDE2.0/tree/master/NewMexico</t>
@@ -754,9 +748,6 @@
   <si>
     <t>if WGW, then Groundwater
 if WSW, then Surface Water</t>
-  </si>
-  <si>
-    <t>NM_C_ + counter</t>
   </si>
   <si>
     <t>COUNTY</t>
@@ -783,13 +774,43 @@
     <t>Surface Ground</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Did some pre-processing to create clean machine readable input file.</t>
+  </si>
+  <si>
+    <t>ose.webmaster@state.nm.us</t>
+  </si>
+  <si>
+    <t>David Hatchner (GIS Manager)</t>
+  </si>
+  <si>
+    <t>505-827-3846</t>
+  </si>
+  <si>
+    <t>https://www.ose.state.nm.us/</t>
+  </si>
+  <si>
+    <t>NMag_WS + counter</t>
+  </si>
+  <si>
+    <t>NMag_RU + counter</t>
+  </si>
+  <si>
+    <t>12/31 + ReportYearCV</t>
+  </si>
+  <si>
+    <t>01/01 +  ReportYearCV</t>
+  </si>
+  <si>
+    <t>NMOSE_Withdrawal</t>
+  </si>
+  <si>
+    <t>Withdrawal</t>
+  </si>
+  <si>
+    <t>'NMOSE_Withdrawal</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1470,6 +1491,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1786,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE91C3C-F676-4E77-8227-802554E4B42D}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1817,7 +1841,7 @@
         <v>217</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1841,7 +1865,7 @@
         <v>219</v>
       </c>
       <c r="B9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1849,7 +1873,7 @@
         <v>220</v>
       </c>
       <c r="B10" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1866,7 +1890,7 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="103"/>
       <c r="B14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1906,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8657C7D5-E8C6-4B34-858E-8D6A434024B4}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2012,8 +2036,12 @@
       <c r="E4" s="84" t="s">
         <v>228</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="85"/>
+      <c r="F4" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="85" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
@@ -2038,10 +2066,14 @@
         <v>15</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="35"/>
+        <v>243</v>
+      </c>
+      <c r="F5" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H5" s="24" t="s">
         <v>11</v>
       </c>
@@ -2065,11 +2097,15 @@
       <c r="D6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="F6" s="86"/>
-      <c r="G6" s="35"/>
+      <c r="F6" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="24" t="s">
         <v>11</v>
       </c>
@@ -2093,11 +2129,15 @@
       <c r="D7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="86" t="s">
+      <c r="E7" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="F7" s="86"/>
-      <c r="G7" s="35"/>
+      <c r="F7" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
@@ -2108,7 +2148,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>115</v>
       </c>
@@ -2121,11 +2161,15 @@
       <c r="D8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="86" t="s">
+      <c r="E8" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="F8" s="86"/>
-      <c r="G8" s="35"/>
+      <c r="F8" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H8" s="24" t="s">
         <v>11</v>
       </c>
@@ -2136,7 +2180,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>118</v>
       </c>
@@ -2149,11 +2193,15 @@
       <c r="D9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="111" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="35"/>
+      <c r="F9" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H9" s="24" t="s">
         <v>11</v>
       </c>
@@ -2162,7 +2210,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>121</v>
       </c>
@@ -2175,11 +2223,15 @@
       <c r="D10" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="111" t="s">
         <v>224</v>
       </c>
-      <c r="F10" s="86"/>
-      <c r="G10" s="35"/>
+      <c r="F10" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H10" s="24" t="s">
         <v>11</v>
       </c>
@@ -2190,7 +2242,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>124</v>
       </c>
@@ -2203,11 +2255,15 @@
       <c r="D11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="111" t="s">
         <v>226</v>
       </c>
-      <c r="F11" s="86"/>
-      <c r="G11" s="35"/>
+      <c r="F11" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
@@ -2231,11 +2287,15 @@
       <c r="D12" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="83" t="s">
+      <c r="E12" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="F12" s="86"/>
-      <c r="G12" s="35"/>
+      <c r="F12" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
@@ -2259,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5623B452-6320-41F9-A4C3-771E435FA050}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,10 +2417,14 @@
         <v>11</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="34"/>
+        <v>254</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
@@ -2384,11 +2448,15 @@
       <c r="D5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="96"/>
+      <c r="E5" s="28">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H5" s="24" t="s">
         <v>11</v>
       </c>
@@ -2415,8 +2483,12 @@
       <c r="E6" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="96"/>
+      <c r="F6" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="24" t="s">
         <v>11</v>
       </c>
@@ -2443,8 +2515,12 @@
       <c r="E7" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="96"/>
+      <c r="F7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
@@ -2469,10 +2545,14 @@
         <v>15</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="96"/>
+        <v>229</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H8" s="24" t="s">
         <v>11</v>
       </c>
@@ -2497,10 +2577,14 @@
         <v>15</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="96"/>
+        <v>229</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H9" s="24" t="s">
         <v>11</v>
       </c>
@@ -2527,8 +2611,12 @@
       <c r="E10" s="28">
         <v>10</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="96"/>
+      <c r="F10" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H10" s="24" t="s">
         <v>11</v>
       </c>
@@ -2555,8 +2643,12 @@
       <c r="E11" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="96"/>
+      <c r="F11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H11" s="24" t="s">
         <v>11</v>
       </c>
@@ -2581,10 +2673,14 @@
         <v>15</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="96"/>
+        <v>255</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
@@ -2609,10 +2705,14 @@
         <v>15</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="96"/>
+        <v>255</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="96" t="s">
+        <v>11</v>
+      </c>
       <c r="H13" s="24" t="s">
         <v>11</v>
       </c>
@@ -2636,8 +2736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203F7812-755D-4EFC-B094-8BF895453DC0}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,7 +2858,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>160</v>
       </c>
@@ -2772,7 +2872,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="95" t="s">
-        <v>161</v>
+        <v>246</v>
       </c>
       <c r="F5" s="86" t="s">
         <v>11</v>
@@ -2790,7 +2890,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>163</v>
       </c>
@@ -2804,7 +2904,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="95" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="F6" s="86" t="s">
         <v>11</v>
@@ -2836,7 +2936,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="95" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F7" s="86" t="s">
         <v>11</v>
@@ -2868,7 +2968,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F8" s="86" t="s">
         <v>11</v>
@@ -2900,7 +3000,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="95" t="s">
-        <v>172</v>
+        <v>248</v>
       </c>
       <c r="F9" s="86" t="s">
         <v>11</v>
@@ -2932,7 +3032,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="95" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F10" s="86" t="s">
         <v>11</v>
@@ -2950,7 +3050,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>177</v>
       </c>
@@ -2964,7 +3064,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="95" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="F11" s="86" t="s">
         <v>11</v>
@@ -2996,7 +3096,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>235</v>
+        <v>197</v>
       </c>
       <c r="F12" s="86" t="s">
         <v>11</v>
@@ -3051,8 +3151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570AF19E-F26B-4187-B7FA-5CACB90F90DE}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3155,7 +3255,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="93"/>
@@ -3323,7 +3423,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="96" t="s">
@@ -3364,7 +3464,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3467,7 +3567,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>11</v>
@@ -3531,7 +3631,7 @@
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="107" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F6" s="97"/>
       <c r="G6" s="100" t="s">
@@ -3561,13 +3661,13 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="107" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F7" s="97" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="98" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H7" s="94" t="s">
         <v>11</v>
@@ -3593,7 +3693,7 @@
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="99" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F8" s="97" t="s">
         <v>11</v>
@@ -3709,7 +3809,7 @@
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="97" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F12" s="97"/>
       <c r="G12" s="100"/>
@@ -3821,8 +3921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E07544-54C6-4298-B1F4-AA27E9BE2694}">
   <dimension ref="A1:K16431"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4107,7 +4207,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G11" s="39"/>
       <c r="H11" s="16" t="s">
@@ -4134,7 +4234,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="105" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="39"/>
@@ -4163,7 +4263,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="47" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="48"/>
@@ -4221,7 +4321,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="107" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F15" s="107" t="s">
         <v>11</v>
@@ -4259,7 +4359,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="109" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="27" t="s">
@@ -4631,7 +4731,7 @@
         <v>15</v>
       </c>
       <c r="E30" s="107" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F30" s="107"/>
       <c r="G30" s="109" t="s">
@@ -4687,10 +4787,12 @@
         <v>15</v>
       </c>
       <c r="E32" s="107" t="s">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="F32" s="107"/>
-      <c r="G32" s="108"/>
+      <c r="G32" s="109" t="s">
+        <v>71</v>
+      </c>
       <c r="H32" s="16" t="s">
         <v>11</v>
       </c>
@@ -4715,10 +4817,12 @@
         <v>15</v>
       </c>
       <c r="E33" s="107" t="s">
-        <v>205</v>
+        <v>253</v>
       </c>
       <c r="F33" s="107"/>
-      <c r="G33" s="108"/>
+      <c r="G33" s="109" t="s">
+        <v>71</v>
+      </c>
       <c r="H33" s="16" t="s">
         <v>11</v>
       </c>

</xml_diff>